<commit_message>
fill date and time
</commit_message>
<xml_diff>
--- a/ExcelEssesntialTraining-Office365/Ch-02-entering-data.xlsx
+++ b/ExcelEssesntialTraining-Office365/Ch-02-entering-data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satya/Data/General-Learning/LearnExcel/ExcelEssesntialTraining-Office365/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC58E667-510A-384B-8EAF-284668F9B804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FFD33-AEDA-C94A-AFCF-1068E18E8792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
+    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
+    <sheet name="DateTime" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Sales</t>
   </si>
@@ -130,6 +131,42 @@
   </si>
   <si>
     <t>see the repitions</t>
+  </si>
+  <si>
+    <t>Use - or / for entering date</t>
+  </si>
+  <si>
+    <t>11-23-2021</t>
+  </si>
+  <si>
+    <t>11/23/2021</t>
+  </si>
+  <si>
+    <t>such as 23-11-2021 or 23/11/2021</t>
+  </si>
+  <si>
+    <t>Date is right aligned</t>
+  </si>
+  <si>
+    <t>Text is right aligned</t>
+  </si>
+  <si>
+    <t>But 11-23-2021 will treat as text not date</t>
+  </si>
+  <si>
+    <t>Use : for time and p  or a for PM or AM</t>
+  </si>
+  <si>
+    <t>24 hrs format</t>
+  </si>
+  <si>
+    <t>ex: 1:34 p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can add days to a date like below </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> such as =A15+100</t>
   </si>
 </sst>
 </file>
@@ -183,10 +220,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDA7B85-F68A-F640-B325-F823EDABA4BF}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -748,4 +788,100 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0D622F-AB8E-0143-8899-5AE766E6E3A2}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="4">
+        <v>0.56527777777777777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>44523</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>44523</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>44523</v>
+      </c>
+      <c r="B15" s="3">
+        <f>A15+100</f>
+        <v>44623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Date, Time, Sum and Average
</commit_message>
<xml_diff>
--- a/ExcelEssesntialTraining-Office365/Ch-02-entering-data.xlsx
+++ b/ExcelEssesntialTraining-Office365/Ch-02-entering-data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satya/Data/General-Learning/LearnExcel/ExcelEssesntialTraining-Office365/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FFD33-AEDA-C94A-AFCF-1068E18E8792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6453A954-1F57-6F46-A876-8BA1053EC89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
+    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
     <sheet name="DateTime" sheetId="2" r:id="rId2"/>
+    <sheet name="Formulas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Sales</t>
   </si>
@@ -167,13 +168,28 @@
   </si>
   <si>
     <t xml:space="preserve"> such as =A15+100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula is =B2-B3 </t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Sum formula is =SUM(B2:G2)</t>
+  </si>
+  <si>
+    <t>Avg formula is =AVERAGE(B2:G2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +199,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,13 +243,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +568,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0D622F-AB8E-0143-8899-5AE766E6E3A2}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,4 +908,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04ACA1A-D318-D84A-985A-A5B87445AC54}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>120</v>
+      </c>
+      <c r="C2" s="6">
+        <v>160</v>
+      </c>
+      <c r="D2" s="6">
+        <v>210</v>
+      </c>
+      <c r="E2" s="6">
+        <v>250</v>
+      </c>
+      <c r="F2" s="6">
+        <v>325</v>
+      </c>
+      <c r="G2" s="6">
+        <v>440</v>
+      </c>
+      <c r="H2" s="6">
+        <f>SUM(B2:G2)</f>
+        <v>1505</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(B2:G2)</f>
+        <v>250.83333333333334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>100</v>
+      </c>
+      <c r="C3" s="6">
+        <v>130</v>
+      </c>
+      <c r="D3" s="6">
+        <v>160</v>
+      </c>
+      <c r="E3" s="6">
+        <v>200</v>
+      </c>
+      <c r="F3" s="6">
+        <v>260</v>
+      </c>
+      <c r="G3" s="6">
+        <v>360</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <f>B2-B3</f>
+        <v>20</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
drag to copy formula column or row wise
</commit_message>
<xml_diff>
--- a/ExcelEssesntialTraining-Office365/Ch-02-entering-data.xlsx
+++ b/ExcelEssesntialTraining-Office365/Ch-02-entering-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satya/Data/General-Learning/LearnExcel/ExcelEssesntialTraining-Office365/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6453A954-1F57-6F46-A876-8BA1053EC89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381592D4-66B8-1845-A4A8-459B3DF4CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Sales</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Avg formula is =AVERAGE(B2:G2)</t>
+  </si>
+  <si>
+    <t>Dragged to copy formula for profits</t>
+  </si>
+  <si>
+    <t>Drag down column to copy avg and sum formula</t>
   </si>
 </sst>
 </file>
@@ -912,10 +918,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04ACA1A-D318-D84A-985A-A5B87445AC54}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,7 +930,7 @@
     <col min="9" max="9" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="6" t="s">
         <v>3</v>
@@ -951,7 +957,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -981,8 +987,11 @@
         <f>AVERAGE(B2:G2)</f>
         <v>250.83333333333334</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1004,9 +1013,16 @@
       <c r="G3" s="6">
         <v>360</v>
       </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" s="6">
+        <f>SUM(B3:G3)</f>
+        <v>1210</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE(B3:G3)</f>
+        <v>201.66666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1014,14 +1030,31 @@
         <f>B2-B3</f>
         <v>20</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="6">
+        <f t="shared" ref="C4:G4" si="0">C2-C3</f>
+        <v>30</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>44</v>
       </c>

</xml_diff>